<commit_message>
Batch processing for 4 scenarios Adding same ending stock rates for the same elevator.
</commit_message>
<xml_diff>
--- a/GCAM_Data/GCAM outputs_20210910.xlsx
+++ b/GCAM_Data/GCAM outputs_20210910.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveutk-my.sharepoint.com/personal/xuzheng_utk_edu/Documents/Scripts/SYBModel/GCAM_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{49E371E1-9069-427F-8ED3-BAC5D35EB541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D58622A-59E2-4E4E-9F7D-08614DB48C2F}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{49E371E1-9069-427F-8ED3-BAC5D35EB541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC97369F-CDCB-45F4-BB22-91DBA0B51A4C}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E81DC82-E771-48D7-8212-60EBA85907A4}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Regional price" sheetId="2" r:id="rId2"/>
     <sheet name="Market supply and demands" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'USA production'!$A$1:$AB$73</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="125">
   <si>
     <t>GCAM_SSP2,date=2021-25-4T21:03:46+20:00</t>
   </si>
@@ -405,9 +408,6 @@
   </si>
   <si>
     <t>Regional supply</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>BasinName</t>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C90626A-C41B-4ECE-816C-F7A7B30DBB68}">
   <dimension ref="A1:AB73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,10 +822,10 @@
         <v>97</v>
       </c>
       <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
         <v>124</v>
-      </c>
-      <c r="F1" t="s">
-        <v>125</v>
       </c>
       <c r="G1">
         <v>1990</v>
@@ -3313,7 +3313,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
         <v>2</v>
@@ -7087,6 +7087,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AB73" xr:uid="{3C90626A-C41B-4ECE-816C-F7A7B30DBB68}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>